<commit_message>
Navbar changes. Squareup implementation. Adding delete button to cart
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\QuinnD\pythonProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E17E1AA1-A961-4860-89AC-7C0CCBFD387F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D341CDF-82CE-4CC6-B396-B422D512C24B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{46D8D163-541B-4806-9D7E-8E234FF6C69B}"/>
+    <workbookView xWindow="-28920" yWindow="915" windowWidth="29040" windowHeight="15720" xr2:uid="{46D8D163-541B-4806-9D7E-8E234FF6C69B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>ID</t>
   </si>
@@ -69,6 +69,45 @@
   </si>
   <si>
     <t>ImageURLs</t>
+  </si>
+  <si>
+    <t>Honda GX160 + MC18 Domestic Acid Pump Viton Seals Carry Frame + 30m Reel</t>
+  </si>
+  <si>
+    <t>This versatile machine is designed to tackle any cleaning task with a selection of nozzles for different spray patterns and an adjustable pressure regulator, to help you clean those hard to reach areas!</t>
+  </si>
+  <si>
+    <t>/static/PetrolPowered/2.jpg</t>
+  </si>
+  <si>
+    <t>Maxflow cold water pressure washer powered by a Honda GX200 petrol engine. Featuring a premium series Comet pump, this machine produces 14 litres per minute water flow at a pressure of 150 bar. Includes chemical pick up hose complete with filter, and adjustable pressure nozzle for chemical application</t>
+  </si>
+  <si>
+    <t>/static/PetrolPowered/3.jpg</t>
+  </si>
+  <si>
+    <t>Maxflow Semi-Industrial Pressure Washer - Honda GX200 14 LPM Low Profile Frame</t>
+  </si>
+  <si>
+    <t>Diesel Washer</t>
+  </si>
+  <si>
+    <t>Maxflow Industrial Pressure Washer - Yanmar L100-V Comet Pump 18 LPM Trolley Frame + Reel</t>
+  </si>
+  <si>
+    <t>Maxflow cold water pressure washer powered by a Yanmar L100 V spec diesel engine. Featuring a HTD type belt driven premium series Comet pump, this machine produces 18 litres per minute water flow at a pressure of 200 bar. Includes reel, chemical pick up hose complete with filter, and adjustable pressure nozzle for chemical application</t>
+  </si>
+  <si>
+    <t>/static/DieselWasher/4.jpg</t>
+  </si>
+  <si>
+    <t>Maxflow Industrial Diesel Hot Pressure Washer - Yanmar L100-V 18 LPM Trolley Frame + Reel</t>
+  </si>
+  <si>
+    <t>Maxflow diesel engine-driven hot wash machine for industrial applications. Produces up to 18 litres per minute at a maximum 200 bar pressure.</t>
+  </si>
+  <si>
+    <t>/static/DieselWasher/5.jpg</t>
   </si>
 </sst>
 </file>
@@ -76,7 +115,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="6" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
+    <numFmt numFmtId="8" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -118,12 +157,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -144,7 +187,7 @@
     <tableColumn id="7" xr3:uid="{0AD4FD58-97CE-4B83-8A06-1C26DFB6FD5A}" name="Department"/>
     <tableColumn id="2" xr3:uid="{F9EB81E3-FF6D-4765-A48C-A602D7D4DE99}" name="Name"/>
     <tableColumn id="3" xr3:uid="{EF0CC762-487D-4F42-9497-195CD3B86D6D}" name="Price"/>
-    <tableColumn id="4" xr3:uid="{6D7FBBFC-519F-42D7-ADFB-1FFA92DBB954}" name="Description"/>
+    <tableColumn id="4" xr3:uid="{6D7FBBFC-519F-42D7-ADFB-1FFA92DBB954}" name="Description" dataDxfId="0"/>
     <tableColumn id="5" xr3:uid="{68B76E19-E8B8-4871-B9CA-25CFCB60B639}" name="ImageURLs"/>
     <tableColumn id="6" xr3:uid="{A4338C0A-DB7E-4514-9BC4-F17D6D17F3FA}" name="Stock"/>
   </tableColumns>
@@ -469,20 +512,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9DF845A-63E6-4F73-B9E1-41616068DD78}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="78.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="141.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="113.28515625" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="141.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -499,7 +542,7 @@
       <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F1" t="s">
@@ -516,7 +559,7 @@
       <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="2">
@@ -529,6 +572,98 @@
         <v>9</v>
       </c>
       <c r="G2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1045</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="2">
+        <v>915</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="2">
+        <v>2625</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="2">
+        <v>7795</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6">
         <v>10</v>
       </c>
     </row>

</xml_diff>